<commit_message>
Working computation of heat transfer area with e-NTU and LMTD methods
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927F812E-39CE-E94D-87FA-D5CD7B99AE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E472FDE-5179-7748-9C8D-3D5DA2C71542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39060" yWindow="500" windowWidth="40880" windowHeight="19040" activeTab="2" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="50420" yWindow="500" windowWidth="13460" windowHeight="20000" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
     <sheet name="Optional Parameters" sheetId="3" r:id="rId2"/>
     <sheet name="Input options" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -67,31 +67,49 @@
     <t>Steam</t>
   </si>
   <si>
-    <t>Thermal Power (kW)</t>
-  </si>
-  <si>
-    <t>Hot Temperature (C)</t>
-  </si>
-  <si>
-    <t>Cold Temperature (C)</t>
-  </si>
-  <si>
-    <t>Mass Flow Rate (kg/s)</t>
-  </si>
-  <si>
-    <t>Tube O.D. (in)</t>
-  </si>
-  <si>
-    <t>Pitch type</t>
-  </si>
-  <si>
-    <t>Tube Pitch Type</t>
-  </si>
-  <si>
-    <t>Triangular</t>
-  </si>
-  <si>
-    <t>Square</t>
+    <t>Primary Hot Temperature (C)</t>
+  </si>
+  <si>
+    <t>Primary Cold Temperature (C)</t>
+  </si>
+  <si>
+    <t>Secondary Hot Temperature (C)</t>
+  </si>
+  <si>
+    <t>Secondary Cold Temperature (C)</t>
+  </si>
+  <si>
+    <t>Primary Mass Flow Rate (kg/s)</t>
+  </si>
+  <si>
+    <t>Secondary Mass Flow Rate (kg/s)</t>
+  </si>
+  <si>
+    <t>Primary Pressure (kPa)</t>
+  </si>
+  <si>
+    <t>Secondary Pressure (kPa)</t>
+  </si>
+  <si>
+    <t>Plate material</t>
+  </si>
+  <si>
+    <t>SS316</t>
+  </si>
+  <si>
+    <t>Hydraulic Diameter (m)</t>
+  </si>
+  <si>
+    <t>Primary Flow Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Secondary Flow Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Plate thickness (m)</t>
+  </si>
+  <si>
+    <t>Thermal Power (MW)</t>
   </si>
 </sst>
 </file>
@@ -229,9 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,23 +564,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="B1" s="11">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -574,35 +594,41 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="11">
+        <v>550</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="11">
+        <v>350</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>6</v>
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -614,7 +640,25 @@
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -631,7 +675,7 @@
           <x14:formula1>
             <xm:f>'Input options'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -641,29 +685,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="12">
-        <v>0.75</v>
+      <c r="A1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -674,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56F1A0A-BA68-8E4B-9018-8BE69B2EE51C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,9 +772,7 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -703,9 +781,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -714,9 +790,7 @@
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">

</xml_diff>

<commit_message>
Add single point Santowax properties. Change input structure to use presssure drop instead of velocity. Add results file for csv results.
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E472FDE-5179-7748-9C8D-3D5DA2C71542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DECF69-793C-E24F-9DF5-5925C3FBA57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50420" yWindow="500" windowWidth="13460" windowHeight="20000" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -97,19 +97,22 @@
     <t>SS316</t>
   </si>
   <si>
-    <t>Hydraulic Diameter (m)</t>
-  </si>
-  <si>
-    <t>Primary Flow Velocity (m/s)</t>
-  </si>
-  <si>
-    <t>Secondary Flow Velocity (m/s)</t>
-  </si>
-  <si>
     <t>Plate thickness (m)</t>
   </si>
   <si>
     <t>Thermal Power (MW)</t>
+  </si>
+  <si>
+    <t>Primary Pressure Drop (kPa)</t>
+  </si>
+  <si>
+    <t>Secondary Pressure Drop (kPa)</t>
+  </si>
+  <si>
+    <t>Flow Length (m)</t>
+  </si>
+  <si>
+    <t>Plate gap (m)</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +581,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="11">
         <v>5</v>
@@ -685,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,34 +702,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="13">
         <v>1E-3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>18</v>
+      <c r="A2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0.5</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -734,16 +737,24 @@
         <v>21</v>
       </c>
       <c r="B5" s="11">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add steam generator cost estimator and conversion cycle efficiency estimator
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DECF69-793C-E24F-9DF5-5925C3FBA57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E45FA-5012-7642-A84A-30D7E9C1C216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50420" yWindow="500" windowWidth="13460" windowHeight="20000" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="34100" windowHeight="20680" activeTab="2" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
-    <sheet name="Optional Parameters" sheetId="3" r:id="rId2"/>
-    <sheet name="Input options" sheetId="2" r:id="rId3"/>
+    <sheet name="HX Parameters" sheetId="3" r:id="rId2"/>
+    <sheet name="Cycle Parameters" sheetId="4" r:id="rId3"/>
+    <sheet name="Input options" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="181029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -64,9 +64,6 @@
     <t>SCO2</t>
   </si>
   <si>
-    <t>Steam</t>
-  </si>
-  <si>
     <t>Primary Hot Temperature (C)</t>
   </si>
   <si>
@@ -112,7 +109,55 @@
     <t>Flow Length (m)</t>
   </si>
   <si>
-    <t>Plate gap (m)</t>
+    <t>Plate Material</t>
+  </si>
+  <si>
+    <t>SS304</t>
+  </si>
+  <si>
+    <t>Allowable pressure loss in the fluid, currently limited to frictional loss.</t>
+  </si>
+  <si>
+    <t>Conduction length between primary and secondary channels.</t>
+  </si>
+  <si>
+    <t>Channel Diameter (m)</t>
+  </si>
+  <si>
+    <t>Diameter of semi-circular channel. Identical between primary and secondary.</t>
+  </si>
+  <si>
+    <t>Step size in meters for use in steam generator modeling</t>
+  </si>
+  <si>
+    <t>Flow length used for non-steam generator modeling</t>
+  </si>
+  <si>
+    <t>Step size (m)</t>
+  </si>
+  <si>
+    <t>HX length lower bound (m)</t>
+  </si>
+  <si>
+    <t>HX length upper bound (m)</t>
+  </si>
+  <si>
+    <t>Lower bound of the heat exchanger length search for steam generator modeling</t>
+  </si>
+  <si>
+    <t>Upper bound of the heat exchanger length search for steam generator modeling</t>
+  </si>
+  <si>
+    <t>Pump/Compressor Efficiency</t>
+  </si>
+  <si>
+    <t>Turbine Efficiency</t>
+  </si>
+  <si>
+    <t>Compression Ratio</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -237,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -246,13 +291,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,7 +315,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -559,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,87 +624,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10">
         <v>20</v>
       </c>
-      <c r="B1" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="11">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="11">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="11">
-        <v>2000</v>
+      <c r="B11" s="10">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -688,85 +734,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="13">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>24</v>
+      <c r="C1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="13">
+      <c r="C2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="10">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADF7FC1C-1A07-FD45-BD27-1BA99C2BB5DA}">
+          <x14:formula1>
+            <xm:f>'Input options'!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D39271-0761-D847-B521-924CF00C9A83}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="10">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="C3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56F1A0A-BA68-8E4B-9018-8BE69B2EE51C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,10 +923,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -792,7 +937,9 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -801,16 +948,17 @@
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Remove cycle efficiency calculation for air brayton cycle. Remove excessive print statements.
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E45FA-5012-7642-A84A-30D7E9C1C216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933A05F5-2F8A-3041-8823-B58EF9FBE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="34100" windowHeight="20680" activeTab="2" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="12780" yWindow="500" windowWidth="34100" windowHeight="20680" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,9 +697,7 @@
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10">
-        <v>20</v>
-      </c>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
@@ -737,7 +735,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D39271-0761-D847-B521-924CF00C9A83}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add flow length iteration to non-steam generator modeling such that outlet conditions are enforced and maximum pressure drop is achieved
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933A05F5-2F8A-3041-8823-B58EF9FBE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388388F-FAF3-F44A-929C-B37BE0E66158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="500" windowWidth="34100" windowHeight="20680" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Cycle Parameters" sheetId="4" r:id="rId3"/>
     <sheet name="Input options" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -106,9 +107,6 @@
     <t>Secondary Pressure Drop (kPa)</t>
   </si>
   <si>
-    <t>Flow Length (m)</t>
-  </si>
-  <si>
     <t>Plate Material</t>
   </si>
   <si>
@@ -128,9 +126,6 @@
   </si>
   <si>
     <t>Step size in meters for use in steam generator modeling</t>
-  </si>
-  <si>
-    <t>Flow length used for non-steam generator modeling</t>
   </si>
   <si>
     <t>Step size (m)</t>
@@ -282,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -296,7 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +622,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="10">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -636,15 +630,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13">
-        <v>390</v>
+      <c r="B3" s="10">
+        <v>630</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -652,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="10">
-        <v>260</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -666,7 +660,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="10">
-        <v>300</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -674,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -682,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="10">
-        <v>295</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -690,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="10">
-        <v>215</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -732,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,91 +747,80 @@
         <v>1E-3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="10">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>30</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="B4" s="10">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="10">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0.2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="10">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="10">
-        <v>2</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +832,7 @@
           <x14:formula1>
             <xm:f>'Input options'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
+          <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -872,7 +855,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="10">
         <v>0.95</v>
@@ -881,7 +864,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="10">
         <v>0.95</v>
@@ -890,10 +873,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10"/>
     </row>
@@ -925,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -955,7 +938,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Remove excess print statements. Update pump and turbine equations. Allow for use of Supercritical CO2. Add pressure drop outputs.
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388388F-FAF3-F44A-929C-B37BE0E66158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46612CF8-964D-3342-A2E9-6E7FBC4D81C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" activeTab="2" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Air</t>
   </si>
   <si>
-    <t>SCO2</t>
-  </si>
-  <si>
     <t>Primary Hot Temperature (C)</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>CarbonDioxide</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="10">
         <v>50</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="10">
         <v>630</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="10">
         <v>300</v>
@@ -651,13 +651,13 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="10">
         <v>3000</v>
@@ -668,12 +668,12 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="10">
         <v>565</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="10">
         <v>275</v>
@@ -689,16 +689,16 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="10">
-        <v>6000</v>
+        <v>25000</v>
       </c>
     </row>
   </sheetData>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,49 +741,49 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="10">
         <v>1E-3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="4">
-        <v>2E-3</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10">
         <v>50</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="10">
         <v>50</v>
@@ -792,35 +792,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="10">
         <v>0.2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="10">
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D39271-0761-D847-B521-924CF00C9A83}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,7 +855,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="10">
         <v>0.95</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="10">
         <v>0.95</v>
@@ -873,10 +873,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="10"/>
     </row>
@@ -890,7 +890,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -927,10 +927,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update iteration method and improve cycle efficiency calculations. Add file for iterating on parameters.
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46612CF8-964D-3342-A2E9-6E7FBC4D81C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D1EB35-62E3-5B4E-AD4A-12BFFC5F428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" activeTab="2" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23080" windowHeight="20680" activeTab="1" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>CarbonDioxide</t>
+  </si>
+  <si>
+    <t>Efficiency of the pump/compressor in the power concersion cycle</t>
+  </si>
+  <si>
+    <t>Efficiency of the turbine</t>
+  </si>
+  <si>
+    <t>Ratio between high and low pressures</t>
+  </si>
+  <si>
+    <t>(Optional) Allows for simplified modeling of a recuperator where the pump inlet temperature is specified and used for pump calculations instead of the secondary cold temperature</t>
+  </si>
+  <si>
+    <t>Secondary Minimum Temperature (C)</t>
   </si>
 </sst>
 </file>
@@ -277,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -291,6 +306,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +626,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -684,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="10">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -698,7 +716,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="10">
-        <v>25000</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -728,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,7 +773,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="4">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>26</v>
@@ -806,7 +824,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="10">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>31</v>
@@ -817,7 +835,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>32</v>
@@ -842,15 +860,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D39271-0761-D847-B521-924CF00C9A83}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,18 +877,22 @@
         <v>33</v>
       </c>
       <c r="B1" s="10">
-        <v>0.95</v>
-      </c>
-      <c r="C1" s="10"/>
+        <v>0.88</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="10">
-        <v>0.95</v>
-      </c>
-      <c r="C2" s="10"/>
+        <v>0.88</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -878,7 +901,18 @@
       <c r="B3" s="10">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented intermediate sodium loop
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgeschke/Documents/gitprojects/MITHEx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\user\tmp\MITHEx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D1EB35-62E3-5B4E-AD4A-12BFFC5F428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E0F376-3BFF-4140-8288-0FDDF2A65BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23080" windowHeight="20680" activeTab="1" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -168,6 +166,12 @@
   </si>
   <si>
     <t>Secondary Minimum Temperature (C)</t>
+  </si>
+  <si>
+    <t>Intermediate Tloss</t>
+  </si>
+  <si>
+    <t>Intermediate dTMultiplier</t>
   </si>
 </sst>
 </file>
@@ -292,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -309,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -615,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,100 +628,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="10">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <f>B3-150</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="10">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="10">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="10">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10">
-        <v>6000</v>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="14">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>
@@ -746,18 +768,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="67.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -768,7 +790,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
@@ -779,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -788,27 +810,27 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="10">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="10">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>28</v>
       </c>
@@ -819,7 +841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
@@ -830,7 +852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
@@ -863,16 +885,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="39.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="39.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -883,7 +905,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
@@ -894,22 +916,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="10">
-        <v>3</v>
+        <v>3.3330000000000002</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="10">
+        <v>32</v>
+      </c>
       <c r="C4" s="13" t="s">
         <v>41</v>
       </c>
@@ -924,17 +948,17 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,7 +969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -956,7 +980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -967,7 +991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -975,7 +999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Adjusted input parameters to match recent optimization studies
</commit_message>
<xml_diff>
--- a/MITHEx_inputs.xlsx
+++ b/MITHEx_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\user\tmp\MITHEx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\user\phd\sc_co2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E0F376-3BFF-4140-8288-0FDDF2A65BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888A448-B6D7-4A9B-A548-2D0F55D25D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
+    <workbookView xWindow="-28920" yWindow="3705" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C84507C0-3159-7149-91A1-7786B2F61E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Description" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Primary Fluid</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>Secondary Minimum Temperature (C)</t>
-  </si>
-  <si>
-    <t>Intermediate Tloss</t>
-  </si>
-  <si>
-    <t>Intermediate dTMultiplier</t>
   </si>
 </sst>
 </file>
@@ -296,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,7 +307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380AF96-944E-E04A-BEFD-544B656D8084}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -723,22 +716,6 @@
       </c>
       <c r="B11" s="10">
         <v>25000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="14">
-        <v>1.04</v>
       </c>
     </row>
   </sheetData>
@@ -768,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34984CC6-669D-944B-B38F-5AD3A5139180}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -795,7 +772,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="4">
-        <v>2E-3</v>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>26</v>
@@ -815,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="10">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>23</v>
@@ -826,7 +803,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="10">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="C5" s="10"/>
     </row>
@@ -865,6 +842,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -948,7 +926,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>